<commit_message>
end fake data et begin API
</commit_message>
<xml_diff>
--- a/Step.XLSX
+++ b/Step.XLSX
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GUEGUEN\Desktop\WSApp\IM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871EEED5-324A-4482-A965-FF8DCC0361DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40C3C51D-69E7-42B9-8263-6F3FEB3414B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -420,7 +420,7 @@
   <dimension ref="A2:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,11 +436,11 @@
       </c>
       <c r="D2">
         <f>(D3*E3+D9*E9+D10*E10+D11*E11+D12*E12+D13*E13)/SUM(D3,D9:D13)</f>
-        <v>7.456445993031359E-2</v>
+        <v>7.8048780487804864E-2</v>
       </c>
       <c r="E2">
         <f>D2*100</f>
-        <v>7.4564459930313589</v>
+        <v>7.8048780487804867</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -453,11 +453,11 @@
       </c>
       <c r="E3" s="2">
         <f>((E4*D4)+(D5*E5)+(D6*E6)+(D7*E7)+D8*E8)/SUM(D4:D8)</f>
-        <v>0.52195121951219514</v>
+        <v>0.54634146341463408</v>
       </c>
       <c r="F3" s="2">
         <f>E3*100</f>
-        <v>52.195121951219512</v>
+        <v>54.634146341463406</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -501,7 +501,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
extract data add to back up data from api
</commit_message>
<xml_diff>
--- a/Step.XLSX
+++ b/Step.XLSX
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GUEGUEN\Desktop\WSApp\IM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40C3C51D-69E7-42B9-8263-6F3FEB3414B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0FE3B37-5100-4969-A85B-DD0B5BE99563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -420,7 +420,7 @@
   <dimension ref="A2:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,11 +436,11 @@
       </c>
       <c r="D2">
         <f>(D3*E3+D9*E9+D10*E10+D11*E11+D12*E12+D13*E13)/SUM(D3,D9:D13)</f>
-        <v>7.8048780487804864E-2</v>
+        <v>0.24564459930313592</v>
       </c>
       <c r="E2">
         <f>D2*100</f>
-        <v>7.8048780487804867</v>
+        <v>24.564459930313593</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -453,11 +453,11 @@
       </c>
       <c r="E3" s="2">
         <f>((E4*D4)+(D5*E5)+(D6*E6)+(D7*E7)+D8*E8)/SUM(D4:D8)</f>
-        <v>0.54634146341463408</v>
+        <v>0.91951219512195126</v>
       </c>
       <c r="F3" s="2">
         <f>E3*100</f>
-        <v>54.634146341463406</v>
+        <v>91.951219512195124</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -490,7 +490,7 @@
         <v>18</v>
       </c>
       <c r="E6" s="1">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -512,7 +512,7 @@
         <v>15</v>
       </c>
       <c r="E8" s="1">
-        <v>0</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -521,6 +521,9 @@
       </c>
       <c r="D9">
         <v>2</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.8</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
begin transform data part
</commit_message>
<xml_diff>
--- a/Step.XLSX
+++ b/Step.XLSX
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GUEGUEN\Desktop\WSApp\IM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0FE3B37-5100-4969-A85B-DD0B5BE99563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96771667-196F-4C3D-9967-869DD6995F2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -419,7 +419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -436,11 +436,11 @@
       </c>
       <c r="D2">
         <f>(D3*E3+D9*E9+D10*E10+D11*E11+D12*E12+D13*E13)/SUM(D3,D9:D13)</f>
-        <v>0.24564459930313592</v>
+        <v>0.26567944250871078</v>
       </c>
       <c r="E2">
         <f>D2*100</f>
-        <v>24.564459930313593</v>
+        <v>26.567944250871079</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -453,11 +453,11 @@
       </c>
       <c r="E3" s="2">
         <f>((E4*D4)+(D5*E5)+(D6*E6)+(D7*E7)+D8*E8)/SUM(D4:D8)</f>
-        <v>0.91951219512195126</v>
+        <v>0.95975609756097546</v>
       </c>
       <c r="F3" s="2">
         <f>E3*100</f>
-        <v>91.951219512195124</v>
+        <v>95.975609756097541</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -490,7 +490,7 @@
         <v>18</v>
       </c>
       <c r="E6" s="1">
-        <v>0.9</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -512,7 +512,7 @@
         <v>15</v>
       </c>
       <c r="E8" s="1">
-        <v>0.9</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -523,7 +523,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="1">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>